<commit_message>
final code ipba 10
</commit_message>
<xml_diff>
--- a/Excel/Time Series Forecasting - Multiplicative 6May2022.xlsx
+++ b/Excel/Time Series Forecasting - Multiplicative 6May2022.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/063bf5775d666102/_YouTube Working Files/Git Time Series/YT_Time_Series_Forecasting/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{849046DB-E208-465A-B047-657A1DEAB550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80F20799-2A60-4AC1-B983-C3CBFE4CC86B}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{849046DB-E208-465A-B047-657A1DEAB550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94A209C0-F51C-49A8-91AC-23C630843DB7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{222811F3-B945-4F38-BB77-4DEABE907094}"/>
+    <workbookView minimized="1" xWindow="37155" yWindow="3780" windowWidth="16380" windowHeight="11250" activeTab="2" xr2:uid="{222811F3-B945-4F38-BB77-4DEABE907094}"/>
   </bookViews>
   <sheets>
     <sheet name="Step0" sheetId="4" r:id="rId1"/>
     <sheet name="Step1" sheetId="1" r:id="rId2"/>
-    <sheet name="Step2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="13" r:id="rId4"/>
-    <sheet name="Step3" sheetId="6" r:id="rId5"/>
-    <sheet name="4ModelOutput" sheetId="8" r:id="rId6"/>
-    <sheet name="Step5" sheetId="9" r:id="rId7"/>
-    <sheet name="Step6" sheetId="10" r:id="rId8"/>
-    <sheet name="OddMA" sheetId="11" r:id="rId9"/>
-    <sheet name="Deseanal" sheetId="12" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId3"/>
+    <sheet name="Step2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="13" r:id="rId5"/>
+    <sheet name="Step3" sheetId="6" r:id="rId6"/>
+    <sheet name="4ModelOutput" sheetId="8" r:id="rId7"/>
+    <sheet name="Step5" sheetId="9" r:id="rId8"/>
+    <sheet name="Step6" sheetId="10" r:id="rId9"/>
+    <sheet name="OddMA" sheetId="11" r:id="rId10"/>
+    <sheet name="Deseanal" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -308,7 +309,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="92">
   <si>
     <t>Year</t>
   </si>
@@ -582,6 +583,9 @@
   <si>
     <t>MA5</t>
   </si>
+  <si>
+    <t>Sales Stationary</t>
+  </si>
 </sst>
 </file>
 
@@ -793,6 +797,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -802,7 +807,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1183,6 +1187,459 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>68000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>98000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>83000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>79000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>104000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-06EA-4FE6-99C9-CE2EBAF49C76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales Stationary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="1">
+                  <c:v>-7000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-14000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-15000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-06EA-4FE6-99C9-CE2EBAF49C76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2069660271"/>
+        <c:axId val="2069657359"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2069660271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2069657359"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2069657359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2069660271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1875,7 +2332,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2161,7 +2618,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2955,7 +3412,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3593,7 +4050,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4231,7 +4688,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4870,6 +5327,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
@@ -5392,6 +5889,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5912,7 +6912,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6415,7 +7415,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6936,7 +7936,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7457,7 +8457,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7978,7 +8978,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8536,6 +9536,177 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9872DBA-67A9-0B47-A13A-E1556B4AAA3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>185070</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>5940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>82470</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>46260</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29050CB-B145-B4A5-0B0C-E6EA8DF841B2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7290720" y="4006440"/>
+            <a:ext cx="3555000" cy="40320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29050CB-B145-B4A5-0B0C-E6EA8DF841B2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7281720" y="3997800"/>
+              <a:ext cx="3572640" cy="57960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>51870</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>11160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>95430</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>67260</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63717766-B2CD-A7F9-688D-6CB0EF0F7346}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7157520" y="2297160"/>
+            <a:ext cx="5529960" cy="1389600"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63717766-B2CD-A7F9-688D-6CB0EF0F7346}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7148880" y="2288160"/>
+              <a:ext cx="5547600" cy="1407240"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8665,7 +9836,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8708,7 +9879,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8749,7 +9920,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8792,7 +9963,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8831,6 +10002,75 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-05-07T06:51:08.563"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">7 1 4972 0 0,'-7'14'7874'0'0,"7"-14"-7743"0"0,22 2 1262 0 0,792 27 2285 0 0,-363-25-3579 0 0,-106 26 78 0 0,32 1-1 0 0,340-30-282 0 0,758-27 922 0 0,-117 36 494 0 0,-751-8-1344 0 0,-123-4 235 0 0,403-1 953 0 0,-773-5-1149 0 0,-28 0 101 0 0,152 8 1 0 0,-222 1 81 0 0,144 12 552 0 0,185-8 1 0 0,281-31-740 0 0,-198 22 994 0 0,-252 5-635 0 0,-159-1-236 0 0,6-1-90 0 0,0 2 0 0 0,0 0 0 0 0,40 8 0 0 0,-68-14-2236 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-05-07T06:51:00.957"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">26 1409 9981 0 0,'-25'-5'3584'0'0,"33"1"-1139"0"0,46-2-237 0 0,-41 5-2065 0 0,203-34 969 0 0,296-87 0 0 0,-326 72-852 0 0,849-153-13 0 0,-922 184-248 0 0,1287-210 1060 0 0,-928 184-927 0 0,-153 21 551 0 0,1058-165 1242 0 0,-585 74-1821 0 0,-446 67 73 0 0,329-28-146 0 0,-210 28-31 0 0,534-63 448 0 0,-948 105-512 0 0,529-59-648 0 0,-557 62-2226 0 0,-11-2-3729 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1085.56">463 2906 7137 0 0,'-29'6'-582'0'0,"-4"7"7789"0"0,33-13-7110 0 0,38-3 1270 0 0,440-91-100 0 0,-163 26-634 0 0,926-115-392 0 0,8 58 225 0 0,163-21-149 0 0,-164-14 1062 0 0,-1022 130-1163 0 0,688-87 432 0 0,-445 53 414 0 0,45-5 493 0 0,48-14-607 0 0,-189 13-2727 0 0,-345 66 23 0 0,27-7-7031 0 0,-49 9 5392 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2202.22">7520 613 6265 0 0,'27'4'3955'0'0,"29"-5"-2585"0"0,-9 0-483 0 0,872-28 2354 0 0,-2-63-2985 0 0,-902 90-249 0 0,248-33 543 0 0,-202 24-296 0 0,1-3 1 0 0,70-26 0 0 0,-129 39-308 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,4-5-1 0 0,-6 5-21 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0-1 0 0,-2-1 1 0 0,-10-10-227 0 0,0 1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 2-1 0 0,-1-1 1 0 0,0 2-1 0 0,-20-7 1 0 0,-9 1 240 0 0,-69-11 0 0 0,81 19 497 0 0,35 9 1095 0 0,17 6 161 0 0,36 11-449 0 0,0-3 0 0 0,77 17 0 0 0,-81-24-899 0 0,-1 2-1 0 0,-1 2 0 0 0,70 32 1 0 0,-115-45-307 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 4 0 0 0,-1-3-27 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-4 4 1 0 0,-8 10-721 0 0,-2 0-1 0 0,0-1 1 0 0,0-1 0 0 0,-2-1 0 0 0,-20 14 0 0 0,-101 55-6282 0 0,127-76 6414 0 0,-44 22-1905 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5106.02">453 3436 4180 0 0,'0'0'144'0'0,"-15"6"10284"0"0,114 25-8286 0 0,122 22 0 0 0,-105-34-1577 0 0,0-6-1 0 0,147 0 1 0 0,369 6 283 0 0,-512-17-831 0 0,-42 1 1 0 0,101-10 0 0 0,-84-4 140 0 0,262-19-291 0 0,676-9 228 0 0,562 12-49 0 0,-1541 27-52 0 0,122 0 15 0 0,1100-11-44 0 0,-496-28 115 0 0,-106 3 39 0 0,-227 38 83 0 0,-76 2-173 0 0,296 14 1287 0 0,-535-4-1148 0 0,170 41 0 0 0,-111-17-283 0 0,-172-32 212 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11057.05">10301 983 9317 0 0,'-2'-22'2166'0'0,"1"15"486"0"0,-3 13-1070 0 0,-12 76-169 0 0,-10 129 1 0 0,14-86-1336 0 0,-61 417-975 0 0,36-310-7308 0 0,31-196 5866 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12161.1">9935 1964 8841 0 0,'9'64'6442'0'0,"4"-8"-5008"0"0,39 109 0 0 0,-47-152-1123 0 0,1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,1-1 1 0 0,15 18-1 0 0,-19-26-294 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,6-3 0 0 0,8-2-531 0 0,0-1 1 0 0,-1-1 0 0 0,1-1 0 0 0,-2-1 0 0 0,1 0-1 0 0,17-14 1 0 0,95-76-7660 0 0,-92 67 5633 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12162.1">10710 2584 12021 0 0,'1'-2'171'0'0,"-1"1"-1"0"0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1-3-1 0 0,0 4-113 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 2 0 0 0,-37 45 87 0 0,-78 121-112 0 0,48-73 96 0 0,47-68-207 0 0,19-28 70 0 0,9-16 37 0 0,125-223 96 0 0,-82 157-64 0 0,-21 32-22 0 0,2 1 0 0 0,2 2 1 0 0,3 1-1 0 0,1 2 0 0 0,47-44 1 0 0,-78 84-41 0 0,-1 0 1 0 0,1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 1-1 0 0,12-4 1 0 0,-16 6 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,2 6 0 0 0,2 4-1 0 0,-1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,-2 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-2-1 1 0 0,1 1-1 0 0,-6 18 0 0 0,-2 4-246 0 0,-1-1-1 0 0,-2-1 1 0 0,-1 0-1 0 0,-25 44 1 0 0,19-44 14 0 0,-2-1 0 0 0,-1-1 0 0 0,-1-1 0 0 0,-2-1 0 0 0,-41 39 0 0 0,16-25-99 0 0,-2-2 0 0 0,-74 45 0 0 0,232-111 432 0 0,52-22 1389 0 0,-33 9-58 0 0,161-28-1 0 0,-265 67-1463 0 0,-17 11 64 0 0,-19 27-351 0 0,5-19-353 0 0,-29 72-7037 0 0,29-65 4931 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14934.55">11464 2548 4220 0 0,'0'20'242'0'0,"1"-1"-1"0"0,1 1 0 0 0,0-1 0 0 0,2 0 0 0 0,0 0 0 0 0,1 0 1 0 0,10 25-1 0 0,-12-36-33 0 0,1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,13 3 1 0 0,-13-5-50 0 0,1 1-1 0 0,-1-1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-2-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,8-14 0 0 0,-1 2 84 0 0,-2-1-1 0 0,0 0 0 0 0,-1-1 1 0 0,-2-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-2 0 0 0 0,6-39 1 0 0,-5 8 1061 0 0,1-94 0 0 0,-8 122-1185 0 0,-1 1 1 0 0,-2-1-1 0 0,0 1 0 0 0,-2-1 1 0 0,0 1-1 0 0,-12-29 1 0 0,17 51-115 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 2 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-2 2 1 0 0,-21 72-18 0 0,22-70-15 0 0,-99 437-527 0 0,-30 121-7060 0 0,114-503 7342 0 0,-72 340-972 0 0,87-395 1252 0 0,-4 47 251 0 0,5-50-237 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,3 2 0 0 0,-2-4 1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-2 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,2-1 1 0 0,28-30 162 0 0,-7 1-161 0 0,-1-2 0 0 0,-1-1 1 0 0,-2 0-1 0 0,24-58 0 0 0,46-154-51 0 0,-71 190 30 0 0,-2-1-1 0 0,-3-1 0 0 0,-3-1 0 0 0,-2 0 0 0 0,2-61 0 0 0,-11 119-3 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,2 0-1 0 0,40 16 55 0 0,-26-10 8 0 0,-6-4 87 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,17-6 0 0 0,-13 2 16 0 0,-1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0-1 1 0 0,-1 1-1 0 0,0-2 0 0 0,16-17 1 0 0,0-6 112 0 0,-2-1 0 0 0,-2-1 0 0 0,-1-1 0 0 0,-1-1 1 0 0,24-61-1 0 0,-13 19 393 0 0,-3-1 0 0 0,-4-1 1 0 0,-3-1-1 0 0,11-89 0 0 0,-32 145-618 0 0,-1 26-52 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-3 4-14 0 0,0 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 7-1 0 0,-103 382 238 0 0,-104 335-7151 0 0,16-174 4069 0 0,189-540 2875 0 0,-13 43 143 0 0,17-55-152 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,3 4 0 0 0,-3-5-6 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,16-17-8 0 0,-16 16 12 0 0,17-21-71 0 0,-1 0 1 0 0,-1-2-1 0 0,-1 0 0 0 0,21-49 1 0 0,32-115-780 0 0,-43 102 820 0 0,-3-2 0 0 0,-4 0 0 0 0,-4-2 0 0 0,-4 1-1 0 0,-2-96 1 0 0,-8 151-21 0 0,-2 1 0 0 0,-12-67 0 0 0,19 109 138 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,14 12 0 0 0,0 0 532 0 0,47 32 0 0 0,-54-43-480 0 0,0-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0-1 0 0,0-2 1 0 0,0 1 0 0 0,1-2 0 0 0,0 0 0 0 0,0-1 0 0 0,25 0-1 0 0,-35-2-140 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1-8-1 0 0,-2 7-12 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-4-9 0 0 0,5 11 4 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,-4-2 0 0 0,6 2 7 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 3 1 0 0,-2 8-14 0 0,0 0 1 0 0,1 1-1 0 0,2 19 0 0 0,-1-20 55 0 0,1 2 178 0 0,0 1 0 0 0,1-1 0 0 0,1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,1 0 1 0 0,1-1 0 0 0,0-1 0 0 0,14 17 0 0 0,-19-24-147 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0-2 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-2-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,10-9-1 0 0,-1 0-98 0 0,0-1 1 0 0,-1-1 0 0 0,-1 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,-1-1-1 0 0,0 0 1 0 0,-1-1 0 0 0,9-20-1 0 0,3-13-470 0 0,32-103-1 0 0,-47 130 362 0 0,2-5-159 0 0,8-48 1 0 0,-16 69 243 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-5-9 0 0 0,7 15 40 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-2 0 0 0 0,0 1 7 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-4 4-1 0 0,-2 3 12 0 0,0 1-1 0 0,0 0 0 0 0,1 0 1 0 0,-11 21-1 0 0,11-13-31 0 0,1 0-1 0 0,0 1 1 0 0,1 0-1 0 0,1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,3 28 1 0 0,1-16 18 0 0,2 0 1 0 0,0-1-1 0 0,2 1 0 0 0,2-1 1 0 0,13 31-1 0 0,-19-53 1 0 0,0-1 0 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,14 8 0 0 0,-8-7 53 0 0,0 0 0 0 0,0-1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1-1 0 0 0,24 0 0 0 0,-15-2 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-2-1 0 0,-1-1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0-2-1 0 0,35-21 1 0 0,-45 22-57 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,6-19 1 0 0,-10 26-29 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-2-10 0 0 0,1 12-36 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,-7-3 1 0 0,7 3 52 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-5 6 0 0 0,4-4 21 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,3 8 0 0 0,2-1 115 0 0,0 0-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,1-2 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,0-1 0 0 0,0-1 0 0 0,1 1 0 0 0,0-2 0 0 0,0 0 0 0 0,1 0 1 0 0,24 6-1 0 0,-22-7 41 0 0,0 0 0 0 0,0-2 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 1 0 0,0-1-1 0 0,-1-1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1-1-1 0 0,21-8 0 0 0,5-14 21 0 0,-38 24-181 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-5 0 0 0,-1 7 5 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-16 5-21 0 0,-15 15-96 0 0,17-7 144 0 0,0 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-11 29 0 0 0,21-44-24 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,13-6 256 0 0,9-9 19 0 0,47-48-335 0 0,-40 34 56 0 0,38-27 0 0 0,-58 49-28 0 0,0 1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 2 0 0 0,-1 0 1 0 0,1 0-1 0 0,19-4 0 0 0,-21 8 25 0 0,1 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 2 1 0 0,14 8 0 0 0,-11-7 6 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,25 7 0 0 0,-27-10 2 0 0,1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1-1 0 0 0,-1 1 0 0 0,11-14 0 0 0,-7-10-131 0 0,-11 30 87 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 2 9 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-17 29-612 0 0,17-27 568 0 0,-5 7 18 0 0,2 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 13-1 0 0,3-22 62 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,6 4 0 0 0,-5-6 34 0 0,-1 1 0 0 0,1-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,3-3 0 0 0,6-4 0 0 0,-1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,16-25 0 0 0,20-49-501 0 0,-8-2-3537 0 0,0 153 1488 0 0,-35-63 2573 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,5-5 0 0 0,11-7 110 0 0,1 0 0 0 0,-2-1 0 0 0,24-22-1 0 0,-26 22-204 0 0,39-40-98 0 0,-55 56 117 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 4 1 0 0,1 3-36 0 0,1-1 76 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,8 13-1 0 0,-9-19-23 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,14-7 15 0 0,-12 7-457 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 1 0 0,6-8-1 0 0,-11 7-1318 0 0,-5 8 907 0 0,-7 13 387 0 0,13-18 507 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 1 1 0 0,14-3 1281 0 0,-13 2-1328 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-5 24 457 0 0,1 1 0 0 0,1 0 0 0 0,2 0 0 0 0,2 39 0 0 0,17 106 1188 0 0,-15-150-1549 0 0,33 381 387 0 0,-32-229-3078 0 0,-4-160 307 0 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9133,7 +10373,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="290" zoomScaleNormal="290" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="A7" sqref="A7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9238,6 +10478,218 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA49CA2-8EB3-4ED1-AE07-BFE54E2254A9}">
+  <dimension ref="D3:F20"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>68000</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>61000</v>
+      </c>
+      <c r="E5" s="2">
+        <f>AVERAGE(D4:D6)</f>
+        <v>69666.666666666672</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>80000</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" ref="E6:E18" si="0">AVERAGE(D5:D7)</f>
+        <v>75333.333333333328</v>
+      </c>
+      <c r="F6" s="2">
+        <f>AVERAGE(D4:D8)</f>
+        <v>74400</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>85000</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>81000</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" ref="F7:F17" si="1">AVERAGE(D5:D9)</f>
+        <v>75200</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>78000</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>78333.333333333328</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>80600</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>72000</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>79333.333333333328</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>83400</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>88000</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>84666.666666666672</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>82400</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>94000</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>87333.333333333328</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>80000</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>83333.333333333328</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
+        <v>86600</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>76000</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>83666.666666666672</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>88600</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>95000</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>89666.666666666672</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>98000</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>92000</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>86200</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>83000</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>86666.666666666672</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>79000</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>87333.333333333328</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
+        <v>92800</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>94333.333333333328</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>104000</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8761320C-1C4A-4423-8E3F-1429667E4D65}">
   <dimension ref="D3:F7"/>
   <sheetViews>
@@ -9265,7 +10717,7 @@
       <c r="D4">
         <v>68000</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="28">
         <v>71735.75380409068</v>
       </c>
       <c r="F4" s="22">
@@ -9276,7 +10728,7 @@
       <c r="D5">
         <v>61000</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="28">
         <v>69687.912606554324</v>
       </c>
       <c r="F5" s="22">
@@ -9287,7 +10739,7 @@
       <c r="D6">
         <v>80000</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="28">
         <v>74732.442706420727</v>
       </c>
       <c r="F6" s="22">
@@ -9298,7 +10750,7 @@
       <c r="D7">
         <v>85000</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="28">
         <v>76657.042250538056</v>
       </c>
       <c r="F7" s="22">
@@ -9315,8 +10767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DA07D5-4067-4300-974B-E9B61B517309}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9325,13 +10777,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -9750,11 +11202,182 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2D9034-1BB6-44FC-A6AF-67B219DCC501}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>68000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>61000</v>
+      </c>
+      <c r="B3" s="2">
+        <f>A3-A2</f>
+        <v>-7000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B18" si="0">A4-A3</f>
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>85000</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>78000</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>-7000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>72000</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>-6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>88000</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>94000</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>-14000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>76000</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>95000</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>98000</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>83000</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>-15000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>79000</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>104000</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DA9F5E-4978-4CC8-9AB3-607969F7620D}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B23"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9799,13 +11422,13 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
       <c r="N5">
         <v>4</v>
       </c>
@@ -9818,10 +11441,10 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="30"/>
       <c r="H6" t="s">
         <v>10</v>
       </c>
@@ -9973,7 +11596,7 @@
         <v>76000</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" ref="G11:G22" si="3">AVERAGE(F11:F12)</f>
+        <f t="shared" ref="G11:G21" si="3">AVERAGE(F11:F12)</f>
         <v>77375</v>
       </c>
       <c r="H11" s="3">
@@ -10429,7 +12052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECB39EF-7309-4B41-B81B-A86D89E6C182}">
   <dimension ref="A1:I18"/>
   <sheetViews>
@@ -10659,12 +12282,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4F9F03-510D-453C-A3C8-DE8A0089C8A2}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10755,10 +12378,10 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="30"/>
       <c r="H7" t="s">
         <v>10</v>
       </c>
@@ -10821,7 +12444,7 @@
         <v>68000</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" ref="I9:I28" si="0">VLOOKUP(D9,$N$2:$O$5,2,FALSE)</f>
+        <f t="shared" ref="I9:I24" si="0">VLOOKUP(D9,$N$2:$O$5,2,FALSE)</f>
         <v>0.94792340491335791</v>
       </c>
       <c r="J9" s="2">
@@ -10858,7 +12481,7 @@
         <v>69687.912606554324</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" ref="K10:K37" si="2">$R$1+$R$2*A10</f>
+        <f t="shared" ref="K10:K28" si="2">$R$1+$R$2*A10</f>
         <v>74078.364157925185</v>
       </c>
     </row>
@@ -11504,7 +13127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BEC6F5-AD1B-444D-8053-1B774B3C287F}">
   <dimension ref="A1:I18"/>
   <sheetViews>
@@ -11738,12 +13361,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D3E6A3-3885-4160-8830-D576A1D5B683}">
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11827,7 +13450,7 @@
       <c r="J6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="L6" s="31" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11835,17 +13458,17 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="30"/>
       <c r="H7" t="s">
         <v>10</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="30"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -11914,7 +13537,7 @@
         <v>72612.569952924343</v>
       </c>
       <c r="L9" s="2">
-        <f>I9*K9</f>
+        <f t="shared" ref="L9:L28" si="2">I9*K9</f>
         <v>68831.154549285435</v>
       </c>
     </row>
@@ -11939,7 +13562,7 @@
         <v>0.8753311401992373</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" ref="J10:J24" si="2">E10/I10</f>
+        <f t="shared" ref="J10:J24" si="3">E10/I10</f>
         <v>69687.912606554324</v>
       </c>
       <c r="K10" s="17">
@@ -11947,7 +13570,7 @@
         <v>74078.364157925185</v>
       </c>
       <c r="L10" s="2">
-        <f>I10*K10</f>
+        <f t="shared" si="2"/>
         <v>64843.098962450968</v>
       </c>
     </row>
@@ -11984,7 +13607,7 @@
         <v>1.0704855495527206</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74732.442706420727</v>
       </c>
       <c r="K11" s="17">
@@ -11992,7 +13615,7 @@
         <v>75544.158362926013</v>
       </c>
       <c r="L11" s="2">
-        <f>I11*K11</f>
+        <f t="shared" si="2"/>
         <v>80868.929880634605</v>
       </c>
     </row>
@@ -12013,15 +13636,15 @@
         <v>85000</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" ref="F12:F23" si="3">AVERAGE(E10:E13)</f>
+        <f t="shared" ref="F12:F23" si="4">AVERAGE(E10:E13)</f>
         <v>76000</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ref="G12:G22" si="4">AVERAGE(F12:F13)</f>
+        <f t="shared" ref="G12:G22" si="5">AVERAGE(F12:F13)</f>
         <v>77375</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ref="H12:H22" si="5">E12/G12</f>
+        <f t="shared" ref="H12:H22" si="6">E12/G12</f>
         <v>1.0985460420032309</v>
       </c>
       <c r="I12" s="16">
@@ -12029,7 +13652,7 @@
         <v>1.1088348507133197</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>76657.042250538056</v>
       </c>
       <c r="K12" s="17">
@@ -12037,7 +13660,7 @@
         <v>77009.952567926855</v>
       </c>
       <c r="L12" s="2">
-        <f>I12*K12</f>
+        <f t="shared" si="2"/>
         <v>85391.319259096999</v>
       </c>
     </row>
@@ -12058,15 +13681,15 @@
         <v>78000</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78750</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79750</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.9780564263322884</v>
       </c>
       <c r="I13" s="16">
@@ -12074,7 +13697,7 @@
         <v>0.94792340491335791</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82285.129363515778</v>
       </c>
       <c r="K13" s="17">
@@ -12082,7 +13705,7 @@
         <v>78475.746772927698</v>
       </c>
       <c r="L13" s="2">
-        <f>I13*K13</f>
+        <f t="shared" si="2"/>
         <v>74388.997084112081</v>
       </c>
     </row>
@@ -12103,15 +13726,15 @@
         <v>72000</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80750</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>81875</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.87938931297709921</v>
       </c>
       <c r="I14" s="16">
@@ -12119,7 +13742,7 @@
         <v>0.8753311401992373</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82254.585371670677</v>
       </c>
       <c r="K14" s="17">
@@ -12127,7 +13750,7 @@
         <v>79941.54097792854</v>
       </c>
       <c r="L14" s="2">
-        <f>I14*K14</f>
+        <f t="shared" si="2"/>
         <v>69975.32021349424</v>
       </c>
     </row>
@@ -12148,15 +13771,15 @@
         <v>88000</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83000</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83250</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.057057057057057</v>
       </c>
       <c r="I15" s="16">
@@ -12164,7 +13787,7 @@
         <v>1.0704855495527206</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82205.686977062796</v>
       </c>
       <c r="K15" s="17">
@@ -12172,7 +13795,7 @@
         <v>81407.335182929382</v>
       </c>
       <c r="L15" s="2">
-        <f>I15*K15</f>
+        <f t="shared" si="2"/>
         <v>87145.375940920683</v>
       </c>
     </row>
@@ -12193,15 +13816,15 @@
         <v>94000</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83500</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84000</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1190476190476191</v>
       </c>
       <c r="I16" s="16">
@@ -12209,7 +13832,7 @@
         <v>1.1088348507133197</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84773.670253536198</v>
       </c>
       <c r="K16" s="17">
@@ -12217,7 +13840,7 @@
         <v>82873.129387930225</v>
       </c>
       <c r="L16" s="2">
-        <f>I16*K16</f>
+        <f t="shared" si="2"/>
         <v>91892.614053011232</v>
       </c>
     </row>
@@ -12238,15 +13861,15 @@
         <v>80000</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>84500</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85375</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.93704245973645683</v>
       </c>
       <c r="I17" s="16">
@@ -12254,7 +13877,7 @@
         <v>0.94792340491335791</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84395.004475400798</v>
       </c>
       <c r="K17" s="17">
@@ -12262,7 +13885,7 @@
         <v>84338.923592931067</v>
       </c>
       <c r="L17" s="2">
-        <f>I17*K17</f>
+        <f t="shared" si="2"/>
         <v>79946.839618938757</v>
       </c>
     </row>
@@ -12283,15 +13906,15 @@
         <v>76000</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>86250</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86750</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.87608069164265134</v>
       </c>
       <c r="I18" s="16">
@@ -12299,7 +13922,7 @@
         <v>0.8753311401992373</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86824.284558985717</v>
       </c>
       <c r="K18" s="17">
@@ -12307,7 +13930,7 @@
         <v>85804.717797931895</v>
       </c>
       <c r="L18" s="2">
-        <f>I18*K18</f>
+        <f t="shared" si="2"/>
         <v>75107.541464537513</v>
       </c>
     </row>
@@ -12328,15 +13951,15 @@
         <v>95000</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87250</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>87625</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0841654778887304</v>
       </c>
       <c r="I19" s="16">
@@ -12344,7 +13967,7 @@
         <v>1.0704855495527206</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88744.775713874624</v>
       </c>
       <c r="K19" s="17">
@@ -12352,7 +13975,7 @@
         <v>87270.512002932737</v>
       </c>
       <c r="L19" s="2">
-        <f>I19*K19</f>
+        <f t="shared" si="2"/>
         <v>93421.822001206747</v>
       </c>
     </row>
@@ -12373,15 +13996,15 @@
         <v>98000</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88000</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88375</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.108910891089109</v>
       </c>
       <c r="I20" s="16">
@@ -12389,7 +14012,7 @@
         <v>1.1088348507133197</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88381.060477090927</v>
       </c>
       <c r="K20" s="17">
@@ -12397,7 +14020,7 @@
         <v>88736.30620793358</v>
       </c>
       <c r="L20" s="2">
-        <f>I20*K20</f>
+        <f t="shared" si="2"/>
         <v>98393.908846925449</v>
       </c>
     </row>
@@ -12418,15 +14041,15 @@
         <v>83000</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88750</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89375</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.92867132867132862</v>
       </c>
       <c r="I21" s="16">
@@ -12434,7 +14057,7 @@
         <v>0.94792340491335791</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87559.817143228327</v>
       </c>
       <c r="K21" s="17">
@@ -12442,7 +14065,7 @@
         <v>90202.100412934422</v>
       </c>
       <c r="L21" s="2">
-        <f>I21*K21</f>
+        <f t="shared" si="2"/>
         <v>85504.682153765403</v>
       </c>
     </row>
@@ -12463,15 +14086,15 @@
         <v>79000</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90000</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90750</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.87052341597796146</v>
       </c>
       <c r="I22" s="16">
@@ -12479,7 +14102,7 @@
         <v>0.8753311401992373</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90251.55894947199</v>
       </c>
       <c r="K22" s="17">
@@ -12487,7 +14110,7 @@
         <v>91667.894617935264</v>
       </c>
       <c r="L22" s="2">
-        <f>I22*K22</f>
+        <f t="shared" si="2"/>
         <v>80239.7627155808</v>
       </c>
     </row>
@@ -12508,7 +14131,7 @@
         <v>100000</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91500</v>
       </c>
       <c r="G23" s="2"/>
@@ -12517,7 +14140,7 @@
         <v>1.0704855495527206</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93415.553383025908</v>
       </c>
       <c r="K23" s="17">
@@ -12525,7 +14148,7 @@
         <v>93133.688822936107</v>
       </c>
       <c r="L23" s="2">
-        <f>I23*K23</f>
+        <f t="shared" si="2"/>
         <v>99698.268061492825</v>
       </c>
     </row>
@@ -12551,7 +14174,7 @@
         <v>1.1088348507133197</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93792.145812423027</v>
       </c>
       <c r="K24" s="17">
@@ -12559,7 +14182,7 @@
         <v>94599.483027936949</v>
       </c>
       <c r="L24" s="2">
-        <f>I24*K24</f>
+        <f t="shared" si="2"/>
         <v>104895.20364083968</v>
       </c>
     </row>
@@ -12577,15 +14200,15 @@
         <v>1</v>
       </c>
       <c r="I25" s="16">
-        <f t="shared" ref="I25:I28" si="6">VLOOKUP(D25,$N$2:$O$5,2,FALSE)</f>
+        <f t="shared" ref="I25:I28" si="7">VLOOKUP(D25,$N$2:$O$5,2,FALSE)</f>
         <v>0.94792340491335791</v>
       </c>
       <c r="K25" s="17">
-        <f t="shared" ref="K25:K28" si="7">$R$1+$R$2*A25</f>
+        <f t="shared" ref="K25:K28" si="8">$R$1+$R$2*A25</f>
         <v>96065.277232937777</v>
       </c>
       <c r="L25" s="2">
-        <f>I25*K25</f>
+        <f t="shared" si="2"/>
         <v>91062.524688592064</v>
       </c>
     </row>
@@ -12603,15 +14226,15 @@
         <v>2</v>
       </c>
       <c r="I26" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.8753311401992373</v>
       </c>
       <c r="K26" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>97531.071437938619</v>
       </c>
       <c r="L26" s="2">
-        <f>I26*K26</f>
+        <f t="shared" si="2"/>
         <v>85371.983966624073</v>
       </c>
     </row>
@@ -12629,15 +14252,15 @@
         <v>3</v>
       </c>
       <c r="I27" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0704855495527206</v>
       </c>
       <c r="K27" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>98996.865642939461</v>
       </c>
       <c r="L27" s="2">
-        <f>I27*K27</f>
+        <f t="shared" si="2"/>
         <v>105974.71412177889</v>
       </c>
     </row>
@@ -12655,15 +14278,15 @@
         <v>4</v>
       </c>
       <c r="I28" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1088348507133197</v>
       </c>
       <c r="K28" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100462.6598479403</v>
       </c>
       <c r="L28" s="2">
-        <f>I28*K28</f>
+        <f t="shared" si="2"/>
         <v>111396.4984347539</v>
       </c>
     </row>
@@ -12678,7 +14301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7077317-5789-49E2-9FD1-ACE8A18EC299}">
   <dimension ref="A1:T28"/>
   <sheetViews>
@@ -12799,21 +14422,21 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="30"/>
       <c r="H7" t="s">
         <v>10</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -13857,216 +15480,4 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA49CA2-8EB3-4ED1-AE07-BFE54E2254A9}">
-  <dimension ref="D3:F20"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="1">
-        <v>68000</v>
-      </c>
-    </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="1">
-        <v>61000</v>
-      </c>
-      <c r="E5" s="2">
-        <f>AVERAGE(D4:D6)</f>
-        <v>69666.666666666672</v>
-      </c>
-    </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="1">
-        <v>80000</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" ref="E6:E18" si="0">AVERAGE(D5:D7)</f>
-        <v>75333.333333333328</v>
-      </c>
-      <c r="F6" s="2">
-        <f>AVERAGE(D4:D8)</f>
-        <v>74400</v>
-      </c>
-    </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="1">
-        <v>85000</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>81000</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" ref="F7:F20" si="1">AVERAGE(D5:D9)</f>
-        <v>75200</v>
-      </c>
-    </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="1">
-        <v>78000</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>78333.333333333328</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="1"/>
-        <v>80600</v>
-      </c>
-    </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="1">
-        <v>72000</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>79333.333333333328</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="1"/>
-        <v>83400</v>
-      </c>
-    </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="1">
-        <v>88000</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>84666.666666666672</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="1"/>
-        <v>82400</v>
-      </c>
-    </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="1">
-        <v>94000</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>87333.333333333328</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="1"/>
-        <v>82000</v>
-      </c>
-    </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="1">
-        <v>80000</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>83333.333333333328</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="1"/>
-        <v>86600</v>
-      </c>
-    </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="1">
-        <v>76000</v>
-      </c>
-      <c r="E13" s="2">
-        <f t="shared" si="0"/>
-        <v>83666.666666666672</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="1"/>
-        <v>88600</v>
-      </c>
-    </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="1">
-        <v>95000</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>89666.666666666672</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="1"/>
-        <v>86400</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="1">
-        <v>98000</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" si="0"/>
-        <v>92000</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="1"/>
-        <v>86200</v>
-      </c>
-    </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="1">
-        <v>83000</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>86666.666666666672</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="1"/>
-        <v>91000</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="1">
-        <v>79000</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>87333.333333333328</v>
-      </c>
-      <c r="F17" s="2">
-        <f t="shared" si="1"/>
-        <v>92800</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="1">
-        <v>100000</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>94333.333333333328</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="1">
-        <v>104000</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>